<commit_message>
Resistències modificades a l'excel
</commit_message>
<xml_diff>
--- a/DOC/component_list.xlsx
+++ b/DOC/component_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projecte_EDD\master\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64706CF9-9313-4F21-B33E-EA533105519F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4D2A99-B907-4CBF-B6E1-C06B1C15B46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -397,13 +397,34 @@
   </si>
   <si>
     <t>2,24 €</t>
+  </si>
+  <si>
+    <t>53,48 €</t>
+  </si>
+  <si>
+    <t>3,12 €</t>
+  </si>
+  <si>
+    <t>0,84€</t>
+  </si>
+  <si>
+    <t>0,85 €</t>
+  </si>
+  <si>
+    <t>0,01 €</t>
+  </si>
+  <si>
+    <t>• Producció de 20.000 peces any • Durada del projecte 3 anys • Nom del projecte: el que sigui... • Empresa ACME</t>
+  </si>
+  <si>
+    <t>Criteris 20000u</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,6 +462,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -468,7 +496,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -491,12 +519,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -506,6 +543,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -794,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,9 +912,11 @@
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="3"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -901,9 +943,11 @@
       <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
+      <c r="H4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="5"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -928,11 +972,13 @@
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -959,9 +1005,11 @@
       <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
+      <c r="H6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -988,9 +1036,11 @@
       <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
+      <c r="H7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="3"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1017,9 +1067,11 @@
       <c r="G8" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
+      <c r="H8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="5"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -1044,11 +1096,13 @@
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="3"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1069,15 +1123,17 @@
       <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
+      <c r="H10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4"/>
       <c r="K10" s="5"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1104,9 +1160,11 @@
       <c r="G11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
+      <c r="H11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="3"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1133,9 +1191,11 @@
       <c r="G12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
+      <c r="H12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4"/>
       <c r="K12" s="5"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1162,9 +1222,11 @@
       <c r="G13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
+      <c r="H13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="3"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1185,15 +1247,17 @@
       <c r="E14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
       <c r="K14" s="5"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -1218,11 +1282,13 @@
         <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="3"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1249,9 +1315,11 @@
       <c r="G16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
+      <c r="H16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="5"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1272,15 +1340,17 @@
       <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="10" t="s">
         <v>119</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
+      <c r="H17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="3"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1307,9 +1377,11 @@
       <c r="G18" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
+      <c r="H18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="4"/>
       <c r="K18" s="5"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1336,9 +1408,11 @@
       <c r="G19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
+      <c r="H19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="3"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1365,9 +1439,11 @@
       <c r="G20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
+      <c r="H20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="4"/>
       <c r="K20" s="5"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -1394,9 +1470,11 @@
       <c r="G21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
+      <c r="H21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1421,11 +1499,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="4"/>
       <c r="K22" s="5"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -1450,11 +1530,13 @@
         <v>6</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="2"/>
       <c r="K23" s="3"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1479,11 +1561,13 @@
         <v>5</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="4"/>
       <c r="K24" s="5"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -1510,9 +1594,11 @@
       <c r="G25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
+      <c r="H25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="3"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1539,9 +1625,11 @@
       <c r="G26" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="5"/>
+      <c r="H26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="4"/>
       <c r="K26" s="5"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -1568,9 +1656,11 @@
       <c r="G27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="3"/>
+      <c r="H27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="3"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -1597,9 +1687,11 @@
       <c r="G28" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="5"/>
+      <c r="H28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="4"/>
       <c r="K28" s="5"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -1626,9 +1718,11 @@
       <c r="G29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
+      <c r="H29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="3"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -1655,9 +1749,11 @@
       <c r="G30" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="5"/>
+      <c r="H30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="5"/>
+      <c r="J30" s="4"/>
       <c r="K30" s="5"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -1684,9 +1780,11 @@
       <c r="G31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
+      <c r="H31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="3"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -1694,7 +1792,7 @@
       <c r="O31" s="2"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>112</v>
       </c>
@@ -1710,87 +1808,93 @@
       <c r="G35" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I35" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
         <v>121</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E31" r:id="rId1" display="https://eu.mouser.com/ProductDetail/Royalohm/TC0550D3302T5G?qs=Wj%2FVkw3K%252BMB5M6MpcX7%252Byw%3D%3D" xr:uid="{35EF156D-EF85-443E-A67A-AEA1B4F3B6F9}"/>
-    <hyperlink ref="D31" r:id="rId2" display="https://eu.mouser.com/datasheet/2/1365/Royalohm_09132021_9__Thin_Film_20200106-2580434.pdf" xr:uid="{EDE9AB5B-EFA8-429F-A7F7-11872BAC6D69}"/>
-    <hyperlink ref="E30" r:id="rId3" display="https://eu.mouser.com/ProductDetail/Royalohm/TC0550F1003T5G?qs=Wj%2FVkw3K%252BMBYxpaKle1zIA%3D%3D" xr:uid="{E5037130-3169-46A8-9D96-351467B60F90}"/>
-    <hyperlink ref="D30" r:id="rId4" display="https://eu.mouser.com/datasheet/2/1365/Royalohm_09132021_9__Thin_Film_20200106-2580434.pdf" xr:uid="{E6974C46-C30C-4C69-9AE0-70C75AC53239}"/>
-    <hyperlink ref="E29" r:id="rId5" display="https://eu.mouser.com/ProductDetail/SEI-Stackpole/RNCP0805JTD10K0?qs=IPgv5n7u5QaJFxYpOecM6A%3D%3D" xr:uid="{1DB00E48-F9E1-4958-B810-CDF887F5210D}"/>
-    <hyperlink ref="D29" r:id="rId6" display="https://eu.mouser.com/datasheet/2/385/SEI_rncp-3077653.pdf" xr:uid="{28924AD1-D03B-4DAA-B480-B8D5959A0209}"/>
-    <hyperlink ref="E28" r:id="rId7" display="https://eu.mouser.com/ProductDetail/Royalohm/TC0550F3300T5F?qs=T%252BzbugeAwjgeSBQZlDaTmA%3D%3D" xr:uid="{7D8357F7-2719-42FC-BB28-0E9F424D0A17}"/>
-    <hyperlink ref="D28" r:id="rId8" display="https://eu.mouser.com/datasheet/2/1365/21-3077223.pdf" xr:uid="{91E179AA-0EDF-4678-A53E-D153610EB025}"/>
-    <hyperlink ref="E27" r:id="rId9" display="https://eu.mouser.com/ProductDetail/Royalohm/TC05W8F1001T5G?qs=ST9lo4GX8V0X3zBMraFh1A%3D%3D" xr:uid="{55DDD406-97F6-4BAD-BD53-67F37AAF6659}"/>
-    <hyperlink ref="D27" r:id="rId10" display="https://eu.mouser.com/datasheet/2/1365/21-3077223.pdf" xr:uid="{0B741CC7-C30C-4ADD-8093-89236029C7A1}"/>
-    <hyperlink ref="E26" r:id="rId11" display="https://www.mouser.es/ProductDetail/Royalohm/CQ05WAF1200T5E?qs=sGAEpiMZZMtlubZbdhIBINZaoL9yqB51WBf9LviuJYE%3D" xr:uid="{A1ABE773-664E-4732-86CC-F2749E1E54FE}"/>
-    <hyperlink ref="D26" r:id="rId12" display="https://www.mouser.es/datasheet/2/1365/10-3358738.pdf" xr:uid="{ECDB5A90-F05A-4B09-8298-3593105B2118}"/>
-    <hyperlink ref="E25" r:id="rId13" display="https://eu.mouser.com/ProductDetail/KEMET/C0805C104M5RAC?qs=VOOUd%252Bza08rWzt4y8eXMuQ%3D%3D" xr:uid="{AF7CA242-553D-491B-912A-A6B98FCC6172}"/>
-    <hyperlink ref="D25" r:id="rId14" display="https://eu.mouser.com/datasheet/2/447/KEM_C1002_X7R_SMD-3316098.pdf" xr:uid="{189FFA01-0511-411E-9C7C-D7425091DD2D}"/>
-    <hyperlink ref="E24" r:id="rId15" display="https://www.mouser.es/ProductDetail/KEMET/C0805C105K3RAC?qs=ycRbFa0SLRQpHhAu2LUs4g%3D%3D" xr:uid="{0FCC25C3-D9DF-4B4B-BCCA-759AE08E3E7C}"/>
-    <hyperlink ref="D24" r:id="rId16" display="https://www.mouser.es/datasheet/2/447/KEM_C1002_X7R_SMD-3316098.pdf" xr:uid="{A4366032-B6AD-4B6E-86E4-651A6FB94739}"/>
-    <hyperlink ref="E23" r:id="rId17" display="https://www.mouser.es/ProductDetail/Wurth-Elektronik/860010372004?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6V%2FBdkDX4IUo%3D" xr:uid="{F6A9C276-C183-40D6-BCE3-88BD25B8FE21}"/>
-    <hyperlink ref="D23" r:id="rId18" display="https://www.we-online.com/components/products/datasheet/860010372004.pdf" xr:uid="{64F47EB5-5E4F-4456-9BA1-C34A10157607}"/>
-    <hyperlink ref="E22" r:id="rId19" display="https://eu.mouser.com/ProductDetail/Wurth-Elektronik/865080540002?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6puNwow3HMPo%3D" xr:uid="{533CB1B0-DAA5-419A-95D2-3F13D2CD595B}"/>
-    <hyperlink ref="D22" r:id="rId20" display="https://www.we-online.com/components/products/datasheet/865080540002.pdf" xr:uid="{B821F353-7CE6-48D6-94F5-881014D70828}"/>
-    <hyperlink ref="E21" r:id="rId21" display="https://eu.mouser.com/ProductDetail/KYOCERA-AVX/KAM31BR81H103KT?qs=Jm2GQyTW%2FbjzijSUJGW%2FJA%3D%3D" xr:uid="{FCBCC094-A86A-46A6-A04F-8AB770EF6DE4}"/>
-    <hyperlink ref="D21" r:id="rId22" display="https://eu.mouser.com/datasheet/2/40/AutoMLCCKAM-3216307.pdf" xr:uid="{1DDA3BEE-8BEB-4DE8-9F38-782C4EF1D470}"/>
-    <hyperlink ref="E20" r:id="rId23" display="https://eu.mouser.com/ProductDetail/Chemi-Con/KTS500B226M76N0T00?qs=yFwz03cOJpkGGSneI4ka0Q%3D%3D" xr:uid="{F1403E85-644F-4A09-AABD-730E2BD5559C}"/>
-    <hyperlink ref="D20" r:id="rId24" display="https://eu.mouser.com/datasheet/2/420/nipc_s_a0010886389_1-2285932.pdf" xr:uid="{A8621DD7-ADE8-4161-821B-4585C6F351B4}"/>
-    <hyperlink ref="E19" r:id="rId25" display="https://eu.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL31B226KPHNNWE?qs=xZ%2FP%252Ba9zWqYr7HUxVtf3Yw%3D%3D" xr:uid="{1B72AA9C-32A9-4E15-805A-9C604B476504}"/>
-    <hyperlink ref="D19" r:id="rId26" display="https://eu.mouser.com/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{1E816C52-9BA8-42BC-B9D3-2C6547D7F852}"/>
-    <hyperlink ref="E18" r:id="rId27" display="https://eu.mouser.com/ProductDetail/KEMET/T491A105K020AT4360?qs=sGAEpiMZZMsh%252B1woXyUXjyEnHz%2F1kG1y%2Fw9r1ZBsrUs%3D" xr:uid="{912B986B-651C-4B42-AD1D-D783DA2E23B2}"/>
-    <hyperlink ref="D18" r:id="rId28" display="https://eu.mouser.com/datasheet/2/447/KEM_T2005_T491-3316937.pdf" xr:uid="{4817F474-4EBE-4CDD-8266-08E93F7F46AA}"/>
-    <hyperlink ref="E17" r:id="rId29" display="https://eu.mouser.com/ProductDetail/CUI-Inc/P783-Q24-S3-S?qs=sPbYRqrBIVl7G8uy4wpmww%3D%3D" xr:uid="{5034372E-BC57-4295-8C83-857784642725}"/>
-    <hyperlink ref="D17" r:id="rId30" display="https://eu.mouser.com/datasheet/2/670/p783_s-1889817.pdf" xr:uid="{A9529BFF-D871-4C13-8588-2BD41905549C}"/>
-    <hyperlink ref="E16" r:id="rId31" display="https://eu.mouser.com/ProductDetail/CUI-Inc/P7803-2000R-S?qs=vvQtp7zwQdObalelOc2Obw%3D%3D" xr:uid="{C2C8252F-E7E4-486F-B1F3-C782844ADC09}"/>
-    <hyperlink ref="D16" r:id="rId32" display="https://eu.mouser.com/datasheet/2/670/p78_2000r_s-3070500.pdf" xr:uid="{575E9712-908F-4D76-9794-3508D883A1FB}"/>
-    <hyperlink ref="E15" r:id="rId33" display="https://www.digikey.es/en/products/detail/panasonic-electronic-components/ESE-22MV21T/1245478" xr:uid="{1099D7E3-52BC-48BC-933F-8C0F98525346}"/>
-    <hyperlink ref="D15" r:id="rId34" display="https://industrial.panasonic.com/cdbs/www-data/pdf/ATB0000/ATB0000C12.pdf" xr:uid="{5F4EE5B4-26DE-4411-8999-75C0DA7655C7}"/>
-    <hyperlink ref="E14" r:id="rId35" display="https://www.transmotec.com/product/dla-12-5-a-50-pot-ip65/" xr:uid="{BECB3E5C-6E02-4679-BC41-66837FBB6182}"/>
-    <hyperlink ref="D14" r:id="rId36" display="https://www.transmotec.com/Download/Catalog/Transmotec-EN-DLA-2022.pdf" xr:uid="{DBBD1B73-3BF9-41B5-ADA0-27797FA69C65}"/>
-    <hyperlink ref="E13" r:id="rId37" display="https://www.digikey.es/en/products/detail/dlp-design-inc/DLP-RFID2/3770244" xr:uid="{D2798009-9944-41A4-9B3D-A0230B356EDE}"/>
-    <hyperlink ref="D13" r:id="rId38" display="https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/5656/DLP-RFID2%28D%29-V2.pdf" xr:uid="{D2B4A64B-5FB8-4162-9305-21CE0BF83744}"/>
-    <hyperlink ref="E12" r:id="rId39" display="https://eu.mouser.com/ProductDetail/WeEn-Semiconductors/BYV10MX-600PQ?qs=QNEnbhJQKvYwaGjd%2F4%252BPWg%3D%3D" xr:uid="{2C07A25C-BDB7-45D5-B385-102D04297979}"/>
-    <hyperlink ref="D12" r:id="rId40" display="https://eu.mouser.com/datasheet/2/848/BYV10MX_600P-2401273.pdf" xr:uid="{66A8F858-446A-4571-882A-468093586CEA}"/>
-    <hyperlink ref="E11" r:id="rId41" display="https://eu.mouser.com/ProductDetail/Diodes-Incorporated/DDZ9699T-7?qs=mQbszxtPdlOBwg08InvD3Q%3D%3D" xr:uid="{8D1DFAF5-5599-444E-9969-36F8DB7A95D1}"/>
-    <hyperlink ref="D11" r:id="rId42" display="https://eu.mouser.com/datasheet/2/115/DIOD_S_A0003550665_1-2542209.pdf" xr:uid="{F6538011-E1AE-4C68-B1F2-EE1AC604FC86}"/>
-    <hyperlink ref="E10" r:id="rId43" display="https://www.mouser.es/ProductDetail/Texas-Instruments/TMCS1123B2AQDVGR?qs=sGAEpiMZZMsPDRSCoHb1X5I%2FjBVAAn8DJGrzHYBTAmBFitJQJPL%2Fbw%3D%3D" xr:uid="{46D5EF1D-824D-444B-B662-7B00E044AE73}"/>
-    <hyperlink ref="D10" r:id="rId44" display="https://www.ti.com/lit/ds/symlink/tmcs1123.pdf?ts=1711707167099&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FTMCS1123%253Futm_source%253Dgoogle%2526utm_medium%253Dcpc%2526utm_campaign%253Dasc-null-null-GPN_EN-cpc-pf-google-wwe_cons%2526utm_content%253DTMCS1123%2526ds_k%253DTMCS1123%2526DCM%253Dyes%2526gad_source%253D1%2526gclid%253DEAIaIQobChMIrdeOip6ZhQMVVSitBh03AwOFEAAYAiAAEgLiCfD_BwE%2526gclsrc%253Daw.ds" xr:uid="{D9CFA107-7C26-4E7A-9C55-1F3291C7142F}"/>
-    <hyperlink ref="E9" r:id="rId45" display="https://www.mouser.es/ProductDetail/Analog-Devices-Maxim-Integrated/MAX22201ATC%2b?qs=stqOd1AaK7%252Bdqi04%2FQHs9Q%3D%3D" xr:uid="{51F98C54-7CA0-49FA-8356-2D3193CDD48A}"/>
-    <hyperlink ref="D9" r:id="rId46" display="https://www.mouser.es/datasheet/2/609/MAX22201_MAX22207-3127854.pdf" xr:uid="{629666F3-4A26-452E-AD59-C00275E54C54}"/>
-    <hyperlink ref="E7" r:id="rId47" display="https://www.mouser.es/ProductDetail/ECS/ECS-3225SMV-080-GP-TR?qs=sGAEpiMZZMtldj7qu1ydrbV2KlGvrVWIvUi3jDw2tLHT0SWfK9heCg%3D%3D" xr:uid="{6DA03D7F-C859-4E92-97B1-5929295CA1C1}"/>
-    <hyperlink ref="D7" r:id="rId48" display="https://www.mouser.es/datasheet/2/122/ECS_3225SMV-1623609.pdf" xr:uid="{C2916E02-F1CB-473D-91D6-5AC4DA0D25C5}"/>
-    <hyperlink ref="E6" r:id="rId49" display="https://www.mouser.es/ProductDetail/Texas-Instruments/TCAN3413DR?qs=sGAEpiMZZMuyKkoWRCJ2WCtyf8MLmt92v%252BoGH2%2F%2FnqAqFeWM6BEVrA%3D%3D" xr:uid="{FC8577AB-10E8-45F3-A4EE-AE09A12E6AAE}"/>
-    <hyperlink ref="D6" r:id="rId50" display="https://www.ti.com/lit/ds/symlink/tcan3414.pdf?ts=1711721678762&amp;ref_url=https%253A%252F%252Fwww.mouser.it%252F" xr:uid="{8BC71C0B-8C31-4D65-A043-9A152E9FC4D8}"/>
-    <hyperlink ref="E5" r:id="rId51" display="https://www.mouser.es/ProductDetail/Nidec-Components/HG37-200-AA-00?qs=Wj%2FVkw3K%252BMBRymxOaiVRvg%3D%3D" xr:uid="{C21388A6-2475-4EFE-BD4C-C0258FE9CD09}"/>
-    <hyperlink ref="D5" r:id="rId52" display="https://www.mouser.es/datasheet/2/972/hg37-2525173.pdf" xr:uid="{DCF6A55D-4B93-4C71-8827-F55E8B5FD1A1}"/>
-    <hyperlink ref="E4" r:id="rId53" display="https://www.digikey.es/en/products/detail/rochester-electronics-llc/LT1528CT-PBF/13481919" xr:uid="{376C3220-DF16-4F6E-AF12-20F002007E42}"/>
-    <hyperlink ref="D4" r:id="rId54" display="https://rocelec.widen.net/view/pdf/nbjrjihvdn/LITCS09222-1.pdf?t.download=true&amp;u=5oefqw" xr:uid="{7D338460-CBA5-4417-B281-6DAF716625ED}"/>
-    <hyperlink ref="E3" r:id="rId55" display="https://www.mouser.es/ProductDetail/Microchip-Technology/PIC32MK0256MCJ048-E-Y8X?qs=vmHwEFxEFR%2FV8wN%2Fdp0noA%3D%3D" xr:uid="{8E6608C9-F0D5-4A88-8253-77AEBEE4BACE}"/>
-    <hyperlink ref="D3" r:id="rId56" display="https://ww1.microchip.com/downloads/aemDocuments/documents/MCU32/ProductDocuments/DataSheets/PIC32MK-General-Purpose-and-Motor-Control-With-CAN-FD-Family-DataSheet-DS60001570D.pdf" xr:uid="{6250C50A-E1B9-447F-89C8-081DB1A26476}"/>
-    <hyperlink ref="D8" r:id="rId57" xr:uid="{E0936839-756F-436D-9384-8570FA0CDEE0}"/>
-    <hyperlink ref="E8" r:id="rId58" xr:uid="{53932EB0-1DEE-4E37-A38D-64E80775301C}"/>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{EDE9AB5B-EFA8-429F-A7F7-11872BAC6D69}"/>
+    <hyperlink ref="E30" r:id="rId2" xr:uid="{E5037130-3169-46A8-9D96-351467B60F90}"/>
+    <hyperlink ref="D30" r:id="rId3" xr:uid="{E6974C46-C30C-4C69-9AE0-70C75AC53239}"/>
+    <hyperlink ref="E29" r:id="rId4" xr:uid="{1DB00E48-F9E1-4958-B810-CDF887F5210D}"/>
+    <hyperlink ref="D29" r:id="rId5" xr:uid="{28924AD1-D03B-4DAA-B480-B8D5959A0209}"/>
+    <hyperlink ref="E28" r:id="rId6" xr:uid="{7D8357F7-2719-42FC-BB28-0E9F424D0A17}"/>
+    <hyperlink ref="D28" r:id="rId7" xr:uid="{91E179AA-0EDF-4678-A53E-D153610EB025}"/>
+    <hyperlink ref="E27" r:id="rId8" xr:uid="{55DDD406-97F6-4BAD-BD53-67F37AAF6659}"/>
+    <hyperlink ref="D27" r:id="rId9" xr:uid="{0B741CC7-C30C-4ADD-8093-89236029C7A1}"/>
+    <hyperlink ref="E26" r:id="rId10" xr:uid="{A1ABE773-664E-4732-86CC-F2749E1E54FE}"/>
+    <hyperlink ref="D26" r:id="rId11" xr:uid="{ECDB5A90-F05A-4B09-8298-3593105B2118}"/>
+    <hyperlink ref="E25" r:id="rId12" display="https://eu.mouser.com/ProductDetail/KEMET/C0805C104M5RAC?qs=VOOUd%252Bza08rWzt4y8eXMuQ%3D%3D" xr:uid="{AF7CA242-553D-491B-912A-A6B98FCC6172}"/>
+    <hyperlink ref="D25" r:id="rId13" display="https://eu.mouser.com/datasheet/2/447/KEM_C1002_X7R_SMD-3316098.pdf" xr:uid="{189FFA01-0511-411E-9C7C-D7425091DD2D}"/>
+    <hyperlink ref="E24" r:id="rId14" display="https://www.mouser.es/ProductDetail/KEMET/C0805C105K3RAC?qs=ycRbFa0SLRQpHhAu2LUs4g%3D%3D" xr:uid="{0FCC25C3-D9DF-4B4B-BCCA-759AE08E3E7C}"/>
+    <hyperlink ref="D24" r:id="rId15" display="https://www.mouser.es/datasheet/2/447/KEM_C1002_X7R_SMD-3316098.pdf" xr:uid="{A4366032-B6AD-4B6E-86E4-651A6FB94739}"/>
+    <hyperlink ref="E23" r:id="rId16" display="https://www.mouser.es/ProductDetail/Wurth-Elektronik/860010372004?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6V%2FBdkDX4IUo%3D" xr:uid="{F6A9C276-C183-40D6-BCE3-88BD25B8FE21}"/>
+    <hyperlink ref="D23" r:id="rId17" display="https://www.we-online.com/components/products/datasheet/860010372004.pdf" xr:uid="{64F47EB5-5E4F-4456-9BA1-C34A10157607}"/>
+    <hyperlink ref="E22" r:id="rId18" display="https://eu.mouser.com/ProductDetail/Wurth-Elektronik/865080540002?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6puNwow3HMPo%3D" xr:uid="{533CB1B0-DAA5-419A-95D2-3F13D2CD595B}"/>
+    <hyperlink ref="D22" r:id="rId19" display="https://www.we-online.com/components/products/datasheet/865080540002.pdf" xr:uid="{B821F353-7CE6-48D6-94F5-881014D70828}"/>
+    <hyperlink ref="E21" r:id="rId20" display="https://eu.mouser.com/ProductDetail/KYOCERA-AVX/KAM31BR81H103KT?qs=Jm2GQyTW%2FbjzijSUJGW%2FJA%3D%3D" xr:uid="{FCBCC094-A86A-46A6-A04F-8AB770EF6DE4}"/>
+    <hyperlink ref="D21" r:id="rId21" display="https://eu.mouser.com/datasheet/2/40/AutoMLCCKAM-3216307.pdf" xr:uid="{1DDA3BEE-8BEB-4DE8-9F38-782C4EF1D470}"/>
+    <hyperlink ref="E20" r:id="rId22" display="https://eu.mouser.com/ProductDetail/Chemi-Con/KTS500B226M76N0T00?qs=yFwz03cOJpkGGSneI4ka0Q%3D%3D" xr:uid="{F1403E85-644F-4A09-AABD-730E2BD5559C}"/>
+    <hyperlink ref="D20" r:id="rId23" display="https://eu.mouser.com/datasheet/2/420/nipc_s_a0010886389_1-2285932.pdf" xr:uid="{A8621DD7-ADE8-4161-821B-4585C6F351B4}"/>
+    <hyperlink ref="E19" r:id="rId24" display="https://eu.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL31B226KPHNNWE?qs=xZ%2FP%252Ba9zWqYr7HUxVtf3Yw%3D%3D" xr:uid="{1B72AA9C-32A9-4E15-805A-9C604B476504}"/>
+    <hyperlink ref="D19" r:id="rId25" display="https://eu.mouser.com/datasheet/2/585/MLCC-1837944.pdf" xr:uid="{1E816C52-9BA8-42BC-B9D3-2C6547D7F852}"/>
+    <hyperlink ref="E18" r:id="rId26" display="https://eu.mouser.com/ProductDetail/KEMET/T491A105K020AT4360?qs=sGAEpiMZZMsh%252B1woXyUXjyEnHz%2F1kG1y%2Fw9r1ZBsrUs%3D" xr:uid="{912B986B-651C-4B42-AD1D-D783DA2E23B2}"/>
+    <hyperlink ref="D18" r:id="rId27" display="https://eu.mouser.com/datasheet/2/447/KEM_T2005_T491-3316937.pdf" xr:uid="{4817F474-4EBE-4CDD-8266-08E93F7F46AA}"/>
+    <hyperlink ref="E17" r:id="rId28" display="https://eu.mouser.com/ProductDetail/CUI-Inc/P783-Q24-S3-S?qs=sPbYRqrBIVl7G8uy4wpmww%3D%3D" xr:uid="{5034372E-BC57-4295-8C83-857784642725}"/>
+    <hyperlink ref="D17" r:id="rId29" display="https://eu.mouser.com/datasheet/2/670/p783_s-1889817.pdf" xr:uid="{A9529BFF-D871-4C13-8588-2BD41905549C}"/>
+    <hyperlink ref="E16" r:id="rId30" display="https://eu.mouser.com/ProductDetail/CUI-Inc/P7803-2000R-S?qs=vvQtp7zwQdObalelOc2Obw%3D%3D" xr:uid="{C2C8252F-E7E4-486F-B1F3-C782844ADC09}"/>
+    <hyperlink ref="D16" r:id="rId31" display="https://eu.mouser.com/datasheet/2/670/p78_2000r_s-3070500.pdf" xr:uid="{575E9712-908F-4D76-9794-3508D883A1FB}"/>
+    <hyperlink ref="E15" r:id="rId32" display="https://www.digikey.es/en/products/detail/panasonic-electronic-components/ESE-22MV21T/1245478" xr:uid="{1099D7E3-52BC-48BC-933F-8C0F98525346}"/>
+    <hyperlink ref="D15" r:id="rId33" display="https://industrial.panasonic.com/cdbs/www-data/pdf/ATB0000/ATB0000C12.pdf" xr:uid="{5F4EE5B4-26DE-4411-8999-75C0DA7655C7}"/>
+    <hyperlink ref="E14" r:id="rId34" display="https://www.transmotec.com/product/dla-12-5-a-50-pot-ip65/" xr:uid="{BECB3E5C-6E02-4679-BC41-66837FBB6182}"/>
+    <hyperlink ref="D14" r:id="rId35" display="https://www.transmotec.com/Download/Catalog/Transmotec-EN-DLA-2022.pdf" xr:uid="{DBBD1B73-3BF9-41B5-ADA0-27797FA69C65}"/>
+    <hyperlink ref="E13" r:id="rId36" display="https://www.digikey.es/en/products/detail/dlp-design-inc/DLP-RFID2/3770244" xr:uid="{D2798009-9944-41A4-9B3D-A0230B356EDE}"/>
+    <hyperlink ref="D13" r:id="rId37" display="https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/5656/DLP-RFID2%28D%29-V2.pdf" xr:uid="{D2B4A64B-5FB8-4162-9305-21CE0BF83744}"/>
+    <hyperlink ref="E12" r:id="rId38" display="https://eu.mouser.com/ProductDetail/WeEn-Semiconductors/BYV10MX-600PQ?qs=QNEnbhJQKvYwaGjd%2F4%252BPWg%3D%3D" xr:uid="{2C07A25C-BDB7-45D5-B385-102D04297979}"/>
+    <hyperlink ref="D12" r:id="rId39" display="https://eu.mouser.com/datasheet/2/848/BYV10MX_600P-2401273.pdf" xr:uid="{66A8F858-446A-4571-882A-468093586CEA}"/>
+    <hyperlink ref="E11" r:id="rId40" display="https://eu.mouser.com/ProductDetail/Diodes-Incorporated/DDZ9699T-7?qs=mQbszxtPdlOBwg08InvD3Q%3D%3D" xr:uid="{8D1DFAF5-5599-444E-9969-36F8DB7A95D1}"/>
+    <hyperlink ref="D11" r:id="rId41" display="https://eu.mouser.com/datasheet/2/115/DIOD_S_A0003550665_1-2542209.pdf" xr:uid="{F6538011-E1AE-4C68-B1F2-EE1AC604FC86}"/>
+    <hyperlink ref="E10" r:id="rId42" display="https://www.mouser.es/ProductDetail/Texas-Instruments/TMCS1123B2AQDVGR?qs=sGAEpiMZZMsPDRSCoHb1X5I%2FjBVAAn8DJGrzHYBTAmBFitJQJPL%2Fbw%3D%3D" xr:uid="{46D5EF1D-824D-444B-B662-7B00E044AE73}"/>
+    <hyperlink ref="D10" r:id="rId43" display="https://www.ti.com/lit/ds/symlink/tmcs1123.pdf?ts=1711707167099&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FTMCS1123%253Futm_source%253Dgoogle%2526utm_medium%253Dcpc%2526utm_campaign%253Dasc-null-null-GPN_EN-cpc-pf-google-wwe_cons%2526utm_content%253DTMCS1123%2526ds_k%253DTMCS1123%2526DCM%253Dyes%2526gad_source%253D1%2526gclid%253DEAIaIQobChMIrdeOip6ZhQMVVSitBh03AwOFEAAYAiAAEgLiCfD_BwE%2526gclsrc%253Daw.ds" xr:uid="{D9CFA107-7C26-4E7A-9C55-1F3291C7142F}"/>
+    <hyperlink ref="E9" r:id="rId44" display="https://www.mouser.es/ProductDetail/Analog-Devices-Maxim-Integrated/MAX22201ATC%2b?qs=stqOd1AaK7%252Bdqi04%2FQHs9Q%3D%3D" xr:uid="{51F98C54-7CA0-49FA-8356-2D3193CDD48A}"/>
+    <hyperlink ref="D9" r:id="rId45" display="https://www.mouser.es/datasheet/2/609/MAX22201_MAX22207-3127854.pdf" xr:uid="{629666F3-4A26-452E-AD59-C00275E54C54}"/>
+    <hyperlink ref="E7" r:id="rId46" display="https://www.mouser.es/ProductDetail/ECS/ECS-3225SMV-080-GP-TR?qs=sGAEpiMZZMtldj7qu1ydrbV2KlGvrVWIvUi3jDw2tLHT0SWfK9heCg%3D%3D" xr:uid="{6DA03D7F-C859-4E92-97B1-5929295CA1C1}"/>
+    <hyperlink ref="D7" r:id="rId47" display="https://www.mouser.es/datasheet/2/122/ECS_3225SMV-1623609.pdf" xr:uid="{C2916E02-F1CB-473D-91D6-5AC4DA0D25C5}"/>
+    <hyperlink ref="E6" r:id="rId48" display="https://www.mouser.es/ProductDetail/Texas-Instruments/TCAN3413DR?qs=sGAEpiMZZMuyKkoWRCJ2WCtyf8MLmt92v%252BoGH2%2F%2FnqAqFeWM6BEVrA%3D%3D" xr:uid="{FC8577AB-10E8-45F3-A4EE-AE09A12E6AAE}"/>
+    <hyperlink ref="D6" r:id="rId49" display="https://www.ti.com/lit/ds/symlink/tcan3414.pdf?ts=1711721678762&amp;ref_url=https%253A%252F%252Fwww.mouser.it%252F" xr:uid="{8BC71C0B-8C31-4D65-A043-9A152E9FC4D8}"/>
+    <hyperlink ref="E5" r:id="rId50" display="https://www.mouser.es/ProductDetail/Nidec-Components/HG37-200-AA-00?qs=Wj%2FVkw3K%252BMBRymxOaiVRvg%3D%3D" xr:uid="{C21388A6-2475-4EFE-BD4C-C0258FE9CD09}"/>
+    <hyperlink ref="D5" r:id="rId51" display="https://www.mouser.es/datasheet/2/972/hg37-2525173.pdf" xr:uid="{DCF6A55D-4B93-4C71-8827-F55E8B5FD1A1}"/>
+    <hyperlink ref="E4" r:id="rId52" display="https://www.digikey.es/en/products/detail/rochester-electronics-llc/LT1528CT-PBF/13481919" xr:uid="{376C3220-DF16-4F6E-AF12-20F002007E42}"/>
+    <hyperlink ref="D4" r:id="rId53" display="https://rocelec.widen.net/view/pdf/nbjrjihvdn/LITCS09222-1.pdf?t.download=true&amp;u=5oefqw" xr:uid="{7D338460-CBA5-4417-B281-6DAF716625ED}"/>
+    <hyperlink ref="E3" r:id="rId54" display="https://www.mouser.es/ProductDetail/Microchip-Technology/PIC32MK0256MCJ048-E-Y8X?qs=vmHwEFxEFR%2FV8wN%2Fdp0noA%3D%3D" xr:uid="{8E6608C9-F0D5-4A88-8253-77AEBEE4BACE}"/>
+    <hyperlink ref="D3" r:id="rId55" display="https://ww1.microchip.com/downloads/aemDocuments/documents/MCU32/ProductDocuments/DataSheets/PIC32MK-General-Purpose-and-Motor-Control-With-CAN-FD-Family-DataSheet-DS60001570D.pdf" xr:uid="{6250C50A-E1B9-447F-89C8-081DB1A26476}"/>
+    <hyperlink ref="D8" r:id="rId56" xr:uid="{E0936839-756F-436D-9384-8570FA0CDEE0}"/>
+    <hyperlink ref="E8" r:id="rId57" xr:uid="{53932EB0-1DEE-4E37-A38D-64E80775301C}"/>
+    <hyperlink ref="E31" r:id="rId58" xr:uid="{E9A2EC3C-F40D-47B8-A768-1C800D200C24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId59"/>
@@ -1798,6 +1902,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="289a0874-0c95-4191-841a-e39351615097" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ED4E95E98BE39645B2A5122B59228C1C" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="befa2a1b9a24cffd904810867b8b238f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="289a0874-0c95-4191-841a-e39351615097" xmlns:ns4="2815469b-4fcf-457f-81f1-22ea46bc5ebe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b584bc5519d0f097e66008559945f81" ns3:_="" ns4:_="">
     <xsd:import namespace="289a0874-0c95-4191-841a-e39351615097"/>
@@ -2026,14 +2138,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="289a0874-0c95-4191-841a-e39351615097" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2044,6 +2148,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCE795B7-2B72-4FC6-9627-DC180CF6477A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="289a0874-0c95-4191-841a-e39351615097"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2815469b-4fcf-457f-81f1-22ea46bc5ebe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCD36479-96DD-494E-99AD-96D567315D91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2062,23 +2183,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCE795B7-2B72-4FC6-9627-DC180CF6477A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="289a0874-0c95-4191-841a-e39351615097"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2815469b-4fcf-457f-81f1-22ea46bc5ebe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59D6F600-C755-4ADE-A4ED-DD771661F606}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Pressupost 1000x i 20000x
</commit_message>
<xml_diff>
--- a/DOC/component_list.xlsx
+++ b/DOC/component_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projecte_EDD\master\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932D4C75-6167-417D-BFF7-CDC6033387CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C65FAA-EAB3-4228-B04E-D9973D14F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="267">
   <si>
     <t>Name</t>
   </si>
@@ -625,6 +625,207 @@
   </si>
   <si>
     <t>1.920,00 €</t>
+  </si>
+  <si>
+    <t>6,11 €</t>
+  </si>
+  <si>
+    <t>6.110,00 €</t>
+  </si>
+  <si>
+    <t>1,18 €</t>
+  </si>
+  <si>
+    <t>1.180,00 €</t>
+  </si>
+  <si>
+    <t>1,04 €</t>
+  </si>
+  <si>
+    <t>1,53 €</t>
+  </si>
+  <si>
+    <t>1.530,00 €</t>
+  </si>
+  <si>
+    <t>90,00 €</t>
+  </si>
+  <si>
+    <t>0,201 €</t>
+  </si>
+  <si>
+    <t>201,00 €</t>
+  </si>
+  <si>
+    <t>35.040,00 €</t>
+  </si>
+  <si>
+    <t>0,25096 €</t>
+  </si>
+  <si>
+    <t>4,43 €</t>
+  </si>
+  <si>
+    <t>4.430,00 €</t>
+  </si>
+  <si>
+    <t>0,101 €</t>
+  </si>
+  <si>
+    <t>101,00 €</t>
+  </si>
+  <si>
+    <t>0,113 €</t>
+  </si>
+  <si>
+    <t>113,00 €</t>
+  </si>
+  <si>
+    <t>1.870,00 €</t>
+  </si>
+  <si>
+    <t>0,069 €</t>
+  </si>
+  <si>
+    <t>69,00 €</t>
+  </si>
+  <si>
+    <t>0,032 €</t>
+  </si>
+  <si>
+    <t>160,00 €</t>
+  </si>
+  <si>
+    <t>0,054 €</t>
+  </si>
+  <si>
+    <t>0,009 €</t>
+  </si>
+  <si>
+    <t>0,018 €</t>
+  </si>
+  <si>
+    <t>324,00 €</t>
+  </si>
+  <si>
+    <t>0,038 €</t>
+  </si>
+  <si>
+    <t>190,00 €</t>
+  </si>
+  <si>
+    <t>0,073 €</t>
+  </si>
+  <si>
+    <t>438,00 €</t>
+  </si>
+  <si>
+    <t>2.080,00 €</t>
+  </si>
+  <si>
+    <t>501,92 €</t>
+  </si>
+  <si>
+    <t>18,00 €</t>
+  </si>
+  <si>
+    <t>0,024 €</t>
+  </si>
+  <si>
+    <t>24,00 €</t>
+  </si>
+  <si>
+    <t>0,074 €</t>
+  </si>
+  <si>
+    <t>148,00 €</t>
+  </si>
+  <si>
+    <t>122.200,00 €</t>
+  </si>
+  <si>
+    <t>1,01 €</t>
+  </si>
+  <si>
+    <t>20.200,00 €</t>
+  </si>
+  <si>
+    <t>1,34 €</t>
+  </si>
+  <si>
+    <t>26.800,00 €</t>
+  </si>
+  <si>
+    <t>0,057 €</t>
+  </si>
+  <si>
+    <t>1.140,00 €</t>
+  </si>
+  <si>
+    <t>0,158 €</t>
+  </si>
+  <si>
+    <t>3.160,00 €</t>
+  </si>
+  <si>
+    <t>700.800,00 €</t>
+  </si>
+  <si>
+    <t>41.600,00 €</t>
+  </si>
+  <si>
+    <t>8.142,40 €</t>
+  </si>
+  <si>
+    <t>0,20356 €</t>
+  </si>
+  <si>
+    <t>4,27 €</t>
+  </si>
+  <si>
+    <t>85.400,00 €</t>
+  </si>
+  <si>
+    <t>1.380,00 €</t>
+  </si>
+  <si>
+    <t>0,089 €</t>
+  </si>
+  <si>
+    <t>1.780,00 €</t>
+  </si>
+  <si>
+    <t>1,83 €</t>
+  </si>
+  <si>
+    <t>36.600,00 €</t>
+  </si>
+  <si>
+    <t>1.080,00 €</t>
+  </si>
+  <si>
+    <t>2.400,00 €</t>
+  </si>
+  <si>
+    <t>6.480,00 €</t>
+  </si>
+  <si>
+    <t>6.360,00 €</t>
+  </si>
+  <si>
+    <t>180,00 €</t>
+  </si>
+  <si>
+    <t>220,00 €</t>
+  </si>
+  <si>
+    <t>0,065 €</t>
+  </si>
+  <si>
+    <t>2.600,00 €</t>
+  </si>
+  <si>
+    <t>0,011 €</t>
   </si>
 </sst>
 </file>
@@ -680,7 +881,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -702,6 +903,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,7 +941,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -750,6 +957,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1040,7 +1250,7 @@
   <dimension ref="B2:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="P22" sqref="P22:P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +1258,7 @@
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
     <col min="8" max="18" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1133,10 +1343,18 @@
       <c r="L3" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="3"/>
+      <c r="M3" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
@@ -1172,10 +1390,10 @@
       <c r="L4" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="5"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="16"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -1211,10 +1429,10 @@
       <c r="L5" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="3"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="16"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -1250,49 +1468,61 @@
       <c r="L6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="5"/>
+      <c r="M6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="15">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="3"/>
+      <c r="M7" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="O7" s="15"/>
+      <c r="P7" s="16"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
@@ -1328,10 +1558,18 @@
       <c r="L8" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="5"/>
+      <c r="M8" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -1367,10 +1605,18 @@
       <c r="L9" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="3"/>
+      <c r="M9" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
@@ -1397,7 +1643,7 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="5"/>
+      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -1433,10 +1679,18 @@
       <c r="L11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="3"/>
+      <c r="M11" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
@@ -1472,10 +1726,18 @@
       <c r="L12" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="5"/>
+      <c r="M12" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
@@ -1511,10 +1773,18 @@
       <c r="L13" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="3"/>
+      <c r="M13" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
@@ -1541,7 +1811,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="5"/>
+      <c r="P14" s="4"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -1577,10 +1847,18 @@
       <c r="L15" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="3"/>
+      <c r="M15" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
@@ -1616,10 +1894,18 @@
       <c r="L16" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="5"/>
+      <c r="M16" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -1646,7 +1932,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
@@ -1682,10 +1968,18 @@
       <c r="L18" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="5"/>
+      <c r="M18" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -1721,10 +2015,18 @@
       <c r="L19" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="3"/>
+      <c r="M19" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
@@ -1760,10 +2062,18 @@
       <c r="L20" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="5"/>
+      <c r="M20" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
@@ -1799,10 +2109,18 @@
       <c r="L21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="3"/>
+      <c r="M21" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
@@ -1838,10 +2156,18 @@
       <c r="L22" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="5"/>
+      <c r="M22" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -1877,10 +2203,18 @@
       <c r="L23" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="3"/>
+      <c r="M23" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
@@ -1916,10 +2250,18 @@
       <c r="L24" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="5"/>
+      <c r="M24" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
@@ -1955,10 +2297,18 @@
       <c r="L25" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="3"/>
+      <c r="M25" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
@@ -1994,10 +2344,18 @@
       <c r="L26" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="5"/>
+      <c r="M26" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
@@ -2033,10 +2391,18 @@
       <c r="L27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="3"/>
+      <c r="M27" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
@@ -2072,10 +2438,18 @@
       <c r="L28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="5"/>
+      <c r="M28" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
@@ -2111,10 +2485,18 @@
       <c r="L29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="3"/>
+      <c r="M29" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
@@ -2150,10 +2532,18 @@
       <c r="L30" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="5"/>
+      <c r="M30" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
@@ -2189,10 +2579,18 @@
       <c r="L31" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="3"/>
+      <c r="M31" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
@@ -2221,7 +2619,9 @@
       <c r="D36" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="E36" s="9" t="s">
+        <v>156</v>
+      </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
@@ -2312,6 +2712,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="289a0874-0c95-4191-841a-e39351615097" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ED4E95E98BE39645B2A5122B59228C1C" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="befa2a1b9a24cffd904810867b8b238f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="289a0874-0c95-4191-841a-e39351615097" xmlns:ns4="2815469b-4fcf-457f-81f1-22ea46bc5ebe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b584bc5519d0f097e66008559945f81" ns3:_="" ns4:_="">
     <xsd:import namespace="289a0874-0c95-4191-841a-e39351615097"/>
@@ -2540,14 +2948,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="289a0874-0c95-4191-841a-e39351615097" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2558,6 +2958,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCE795B7-2B72-4FC6-9627-DC180CF6477A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="289a0874-0c95-4191-841a-e39351615097"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2815469b-4fcf-457f-81f1-22ea46bc5ebe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCD36479-96DD-494E-99AD-96D567315D91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2576,23 +2993,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCE795B7-2B72-4FC6-9627-DC180CF6477A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="289a0874-0c95-4191-841a-e39351615097"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2815469b-4fcf-457f-81f1-22ea46bc5ebe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59D6F600-C755-4ADE-A4ED-DD771661F606}">
   <ds:schemaRefs>

</xml_diff>